<commit_message>
added sbukid dataset files and evaluation details
</commit_message>
<xml_diff>
--- a/experiments.server/SBUKId.sVO.Checkpoints.Analysis.xlsx
+++ b/experiments.server/SBUKId.sVO.Checkpoints.Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0ut51d3r5.17711\_hlu.Projects.Data\mpgrResources\e2eET-Skeleton-Based-HGR-Using-Data-Level-Fusion\experiments.server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D8641D-E3B5-4E0A-A2EE-BCA3202A6B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A281457-030B-4305-8F7D-AF0B614D3BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BQQFoQzjq05UrbyxlB1SzAjMfv+h/bfbQW090FhX5j1OQuz6Kd0l1el7NVwtBbdmtA2Dr1L4y11AQvPNhtBAlw==" workbookSaltValue="+/FuigNQ8Er61Dsf5IlxNg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3024" yWindow="1224" windowWidth="20748" windowHeight="15576" activeTab="1" xr2:uid="{EBCD7E69-19C3-4832-9770-73C757D4C723}"/>
@@ -18,29 +18,29 @@
     <sheet name="pvTable" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">pvTable!$H$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">pvTable!$I$16</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">pvTable!$M$17:$M$21</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">pvTable!$N$16</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">pvTable!$N$17:$N$21</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">pvTable!$O$16</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">pvTable!$O$17:$O$21</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">pvTable!$C$16</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">pvTable!$C$17:$C$21</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">pvTable!$D$16</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">pvTable!$D$17:$D$21</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">pvTable!$E$16</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">pvTable!$I$17:$I$21</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">pvTable!$E$17:$E$21</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">pvTable!$F$16</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">pvTable!$F$17:$F$21</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">pvTable!$J$16</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">pvTable!$J$17:$J$21</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">pvTable!$K$16</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">pvTable!$K$17:$K$21</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">pvTable!$L$16</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">pvTable!$L$17:$L$21</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">pvTable!$M$16</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">pvTable!$C$16</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">pvTable!$C$17:$C$21</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">pvTable!$I$17:$I$21</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">pvTable!$J$16</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">pvTable!$J$17:$J$21</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">pvTable!$K$16</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">pvTable!$K$17:$K$21</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">pvTable!$L$16</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">pvTable!$L$17:$L$21</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">pvTable!$M$16</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">pvTable!$M$17:$M$21</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">pvTable!$N$16</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">pvTable!$D$16</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">pvTable!$N$17:$N$21</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">pvTable!$O$16</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">pvTable!$O$17:$O$21</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">pvTable!$D$17:$D$21</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">pvTable!$E$16</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">pvTable!$E$17:$E$21</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">pvTable!$F$16</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">pvTable!$F$17:$F$21</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">pvTable!$H$23</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">pvTable!$I$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -88,10 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="99">
-  <si>
-    <t>Dynamic Hand Gestures Classification | all Datasets | raw Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="86">
   <si>
     <t>e_secret</t>
   </si>
@@ -348,43 +345,7 @@
     <t>sVOs/Folds Average</t>
   </si>
   <si>
-    <t>[699c]</t>
-  </si>
-  <si>
-    <t>Random.70:30</t>
-  </si>
-  <si>
-    <t>[1fcc]</t>
-  </si>
-  <si>
-    <t>[8e28]</t>
-  </si>
-  <si>
-    <t>[5f33]</t>
-  </si>
-  <si>
-    <t>[8dec]</t>
-  </si>
-  <si>
-    <t>[a747]</t>
-  </si>
-  <si>
-    <t>0.9059 -&gt;- [699c]-040923.1737-SBUKID.3d-8G-[topdown]</t>
-  </si>
-  <si>
-    <t>0.9765 -&gt;- [1fcc]-040923.1800-SBUKID.3d-8G-[frontto]</t>
-  </si>
-  <si>
-    <t>0.9529 -&gt;- [8e28]-040923.1822-SBUKID.3d-8G-[frontaway]</t>
-  </si>
-  <si>
-    <t>0.4471 -&gt;- [5f33]-040923.1846-SBUKID.3d-8G-[sideright]</t>
-  </si>
-  <si>
-    <t>0.6471 -&gt;- [8dec]-040923.1909-SBUKID.3d-8G-[sideleft]</t>
-  </si>
-  <si>
-    <t>0.6941 -&gt;- [a747]-040923.2004-SBUKID.3d-8G-[custom]</t>
+    <t>Dynamic Human Action Classification | SBUKId Dataset | raw Data</t>
   </si>
 </sst>
 </file>
@@ -1509,55 +1470,55 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="2">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="3">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
         <cx:f>_xlchart.v1.8</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="4">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
-    <cx:data id="5">
+    <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
+    <cx:data id="2">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.14</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.16</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.18</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.20</cx:f>
+      </cx:numDim>
+    </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1567,7 +1528,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{DF9F2591-AF3E-4599-89E8-5FB488372D9F}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>[custom]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1579,7 +1540,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F385C401-69BB-429F-8882-0AB9F07943AC}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.11</cx:f>
               <cx:v>[frontaway]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1591,7 +1552,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B32506B4-33E5-4AE0-B697-73A65BDA0723}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>[frontto]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1603,7 +1564,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A4AB2EAE-64CC-4BAC-9138-66A7FF203FD2}" formatIdx="3">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.15</cx:f>
               <cx:v>[sideleft]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1615,7 +1576,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{663AF9EF-C447-459E-B72E-E9733C4C8BC7}" formatIdx="4">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.17</cx:f>
               <cx:v>[sideright]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1627,7 +1588,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{0EEA5FDB-A94B-44A4-AEE6-344FD149BDA1}" formatIdx="5">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:f>_xlchart.v1.19</cx:f>
               <cx:v>[topdown]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1639,7 +1600,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-C037-4245-BA3B-C4F3F2BAA171}" formatIdx="7">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.21</cx:f>
               <cx:v>sVOs/Folds Average</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1716,22 +1677,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.22</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1741,7 +1702,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-5ADB-47F7-A588-BAC711539950}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.15</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>[frontaway]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1753,7 +1714,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000002-5ADB-47F7-A588-BAC711539950}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>[frontto]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1765,7 +1726,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000003-5ADB-47F7-A588-BAC711539950}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>[topdown]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1777,7 +1738,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000004-5ADB-47F7-A588-BAC711539950}" formatIdx="3">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.21</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>sVOs/Folds Average</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3726,7 +3687,25 @@
     </format>
   </formats>
   <conditionalFormats count="7">
-    <conditionalFormat priority="7">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="5" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -3734,7 +3713,70 @@
               <x v="0"/>
             </reference>
             <reference field="4" count="1" selected="0">
+              <x v="5"/>
+            </reference>
+            <reference field="5" count="5">
               <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="5" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="4">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="5" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="2"/>
             </reference>
             <reference field="5" count="5">
               <x v="0"/>
@@ -3768,7 +3810,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="5">
+    <conditionalFormat priority="7">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -3776,87 +3818,6 @@
               <x v="0"/>
             </reference>
             <reference field="4" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="4">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="4" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="3">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="4" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="4" count="1" selected="0">
-              <x v="5"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="5" count="5">
@@ -4205,7 +4166,25 @@
     </format>
   </formats>
   <conditionalFormats count="7">
-    <conditionalFormat priority="26">
+    <conditionalFormat priority="8">
+      <pivotAreas count="1">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="5" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="9">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -4213,7 +4192,70 @@
               <x v="0"/>
             </reference>
             <reference field="4" count="1" selected="0">
+              <x v="5"/>
+            </reference>
+            <reference field="5" count="5">
               <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="10">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="5" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="11">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="5" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="12">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="4" count="1" selected="0">
+              <x v="2"/>
             </reference>
             <reference field="5" count="5">
               <x v="0"/>
@@ -4247,7 +4289,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="12">
+    <conditionalFormat priority="26">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -4255,87 +4297,6 @@
               <x v="0"/>
             </reference>
             <reference field="4" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="11">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="4" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="10">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="4" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="9">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="4" count="1" selected="0">
-              <x v="5"/>
-            </reference>
-            <reference field="5" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="8">
-      <pivotAreas count="1">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="5" count="5">
@@ -4659,9 +4620,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B032A6-999D-408E-8A1B-05DA89C8BCCF}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4676,7 +4639,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4685,964 +4648,808 @@
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="J4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>30923.221600000001</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G5" s="2">
         <v>0.92730000000000001</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>30923.2238</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>30923.225900000001</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G7" s="2">
         <v>0.96360000000000001</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>30923.232100000001</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G8" s="2">
         <v>0.70909999999999995</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <v>30923.234199999999</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G9" s="2">
         <v>0.8</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>40923.0003</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G10" s="2">
         <v>0.78180000000000005</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <v>40923.002500000002</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2">
         <v>0.90380000000000005</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
         <v>40923.004500000003</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2">
         <v>0.90380000000000005</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
         <v>40923.010499999997</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="2">
         <v>0.92310000000000003</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2">
         <v>40923.061399999999</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="2">
         <v>0.75</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
         <v>40923.063600000001</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="2">
         <v>0.73080000000000001</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>40923.065699999999</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="2">
         <v>0.73080000000000001</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
         <v>40923.072</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2">
         <v>0.875</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>40923.074200000003</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2">
         <v>0.94640000000000002</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2">
         <v>40923.080399999999</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="2">
         <v>0.92859999999999998</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
         <v>40923.082699999999</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2">
         <v>0.71430000000000005</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2">
         <v>40923.084900000002</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2">
         <v>0.75</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2">
         <v>40923.094100000002</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2">
         <v>0.66069999999999995</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <v>40923.100400000003</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="2">
         <v>0.85189999999999999</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2">
         <v>40923.102700000003</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="2">
         <v>0.92589999999999995</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2">
         <v>40923.104899999998</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="2">
         <v>0.94440000000000002</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2">
         <v>40923.111199999999</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="2">
         <v>0.81479999999999997</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2">
         <v>40923.113499999999</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="2">
         <v>0.77780000000000005</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2">
         <v>40923.1158</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="2">
         <v>0.81479999999999997</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2">
         <v>40923.122199999998</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G29" s="2">
         <v>0.89229999999999998</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="2">
         <v>40923.124499999998</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E30" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G30" s="2">
         <v>0.90769999999999995</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2">
         <v>40923.130700000002</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E31" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G31" s="2">
         <v>0.9385</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="2">
         <v>40923.132899999997</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G32" s="2">
         <v>0.53849999999999998</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="2">
         <v>40923.1351</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E33" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G33" s="2">
         <v>0.6</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2">
         <v>40923.141499999998</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G34" s="2">
         <v>0.69230000000000003</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="2">
-        <v>40923.173699999999</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G35" s="2">
-        <v>0.90590000000000004</v>
-      </c>
-      <c r="J35" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="2">
-        <v>40923.18</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0.97650000000000003</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="2">
-        <v>40923.182200000003</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0.95289999999999997</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="2">
-        <v>40923.184600000001</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="2">
-        <v>0.4471</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="2">
-        <v>40923.190900000001</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G39" s="2">
-        <v>0.64710000000000001</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="2">
-        <v>40923.200400000002</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="2">
-        <v>0.69410000000000005</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -5654,7 +5461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33084B1E-58E2-48B3-BAB2-E067DDE9D39F}">
   <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L29" sqref="L28:L29"/>
     </sheetView>
   </sheetViews>
@@ -5674,19 +5481,19 @@
     <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="40"/>
       <c r="E3" s="40"/>
       <c r="F3" s="41"/>
       <c r="H3" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
@@ -5697,48 +5504,48 @@
     </row>
     <row r="4" spans="2:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="E4" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="N4" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="46">
         <v>0.96360000000000001</v>
@@ -5753,7 +5560,7 @@
         <v>0.96363333333333345</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="15">
         <v>0.78180000000000005</v>
@@ -5779,7 +5586,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="46">
         <v>0.92310000000000003</v>
@@ -5794,7 +5601,7 @@
         <v>0.91023333333333334</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="15">
         <v>0.73080000000000001</v>
@@ -5820,7 +5627,7 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="46">
         <v>0.92859999999999998</v>
@@ -5835,7 +5642,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="15">
         <v>0.66069999999999995</v>
@@ -5861,7 +5668,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="46">
         <v>0.94440000000000002</v>
@@ -5876,7 +5683,7 @@
         <v>0.90739999999999998</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="15">
         <v>0.81479999999999997</v>
@@ -5902,7 +5709,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="46">
         <v>0.9385</v>
@@ -5917,7 +5724,7 @@
         <v>0.91283333333333339</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I9" s="15">
         <v>0.69230000000000003</v>
@@ -5943,7 +5750,7 @@
     </row>
     <row r="10" spans="2:15" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="48">
         <v>0.93964000000000003</v>
@@ -5958,7 +5765,7 @@
         <v>0.92215333333333349</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I10" s="22">
         <v>0.73607999999999996</v>

</xml_diff>